<commit_message>
correct variables in character pages
</commit_message>
<xml_diff>
--- a/input/characters_withLakonAndQuantitativeData.xlsx
+++ b/input/characters_withLakonAndQuantitativeData.xlsx
@@ -223,7 +223,7 @@
     <t>Rungsit (pertapa)</t>
   </si>
   <si>
-    <t>Semar_Boyong_(Wahyu_Katetreman),Wahyu_Topeng_Waja,Semar_Mantu,Semar_mBangun_Kayangan,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Wahyu_Cakraningrat,Wahyu_Kembar</t>
+    <t>Semar_Boyong_(Wahyu_Katetreman),Wahyu_Topeng_Waja,Semar_Mantu,Semar_mBangun_Kayangan,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Wahyu_Cakraningrat,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Abiyasa</t>
@@ -364,7 +364,7 @@
     <t>bharat, cenguk</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Semar_Boyong_(Wahyu_Katetreman),Wahyu_Topeng_Waja,Semar_Mantu,Wahyu_Makutharama,Semar_mBangun_Kayangan,Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat</t>
+    <t>Narayana_Kridha_Brata,Semar_Boyong_(Wahyu_Katetreman),Wahyu_Topeng_Waja,Semar_Mantu,Wahyu_Makutharama,Semar_mBangun_Kayangan,Prabu_Bimasakti,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat</t>
   </si>
   <si>
     <t>Antaboga</t>
@@ -421,7 +421,7 @@
     <t>Barata:x; Arjuna:x</t>
   </si>
   <si>
-    <t>Semar_Boyong_(Wahyu_Katetreman),Semar_Boyong_(Wahyu_Katentreman)</t>
+    <t>Semar_Boyong_(Wahyu_Katetreman)</t>
   </si>
   <si>
     <t>Antareja</t>
@@ -577,7 +577,7 @@
     <t>Gendreh</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Semar_Mantu,Wahyu_Makutharama,Semar_Barang_Jantur,Semar_mBangun_Kayangan,Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
+    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Semar_Mantu,Wahyu_Makutharama,Semar_Barang_Jantur,Semar_mBangun_Kayangan,Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Asmarawati</t>
@@ -688,7 +688,7 @@
     <t>Banyak, Gillut</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Wahyu_Topeng_Waja,Semar_Mantu,Semar_Barang_Jantur,Semar_mBangun_Kayangan,Basudewa_Grogol,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Kunthi_Pilih_(Lahiripun_Adipati_Karna),Babad_Wanamarta,Wahyu_Kaprawiran,Bandung_Nagasewu,Gatotkaca_Lahir,Wahyu_Kembar</t>
+    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Wahyu_Topeng_Waja,Semar_Mantu,Semar_Barang_Jantur,Semar_mBangun_Kayangan,Basudewa_Grogol,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Prabu_Bimasakti,Kunthi_Pilih_(Lahiripun_Adipati_Karna),Babad_Wanamarta,Wahyu_Kaprawiran,Bandung_Nagasewu,Gatotkaca_Lahir,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Baladewa</t>
@@ -736,7 +736,7 @@
     <t>Geger</t>
   </si>
   <si>
-    <t>Semar_Boyong_(Wahyu_Katetreman),Wahyu_Topeng_Waja,Semar_Mantu,Semar_Barang_Jantur,Basudewa_Grogol,Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Gatotkaca_Lahir</t>
+    <t>Semar_Boyong_(Wahyu_Katetreman),Wahyu_Topeng_Waja,Semar_Mantu,Semar_Barang_Jantur,Basudewa_Grogol,Prabu_Bimasakti,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Gatotkaca_Lahir</t>
   </si>
   <si>
     <t>Banowati</t>
@@ -775,7 +775,7 @@
     <t>Lanyap</t>
   </si>
   <si>
-    <t>Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Wahyu_Makutharama,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Sudamala,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat,Wahyu_Kembar</t>
+    <t>Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Wahyu_Makutharama,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Sudamala,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Bantala</t>
@@ -1475,7 +1475,7 @@
     <t>626-629</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Wahyu_Makutharama,Semar_mBangun_Kayangan,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat,Wahyu_Kembar</t>
+    <t>Narayana_Kridha_Brata,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Wahyu_Makutharama,Semar_mBangun_Kayangan,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Duryudana</t>
@@ -1523,7 +1523,7 @@
     <t>No wanda (Gembleng = material)</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Semar_Mantu,Wahyu_Makutharama,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat,Wahyu_Kembar</t>
+    <t>Narayana_Kridha_Brata,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Semar_Mantu,Wahyu_Makutharama,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Erawati</t>
@@ -1668,7 +1668,7 @@
     <t>Dukun</t>
   </si>
   <si>
-    <t>Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Wahyu_Topeng_Waja,Semar_Mantu,Wahyu_Makutharama,Semar_mBangun_Kayangan,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Gatotkaca_Lahir,Wahyu_Kembar</t>
+    <t>Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Wahyu_Topeng_Waja,Semar_Mantu,Wahyu_Makutharama,Semar_mBangun_Kayangan,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Prabu_Bimasakti,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Gatotkaca_Lahir,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Gendara</t>
@@ -1935,7 +1935,7 @@
     <t>138-139</t>
   </si>
   <si>
-    <t>Semar_Boyong_(Wahyu_Katetreman),Semar_mBangun_Kayangan,Semar_Boyong_(Wahyu_Katentreman)</t>
+    <t>Semar_Boyong_(Wahyu_Katetreman),Semar_mBangun_Kayangan</t>
   </si>
   <si>
     <t>Kangsa</t>
@@ -2010,7 +2010,7 @@
     <t>Banteng, Pamuk</t>
   </si>
   <si>
-    <t>Semar_Boyong_(Wahyu_Katetreman),Dewa_Ruci,Wahyu_Makutharama,Semar_Boyong_(Wahyu_Katentreman),Kunthi_Pilih_(Lahiripun_Adipati_Karna),Sudamala,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
+    <t>Semar_Boyong_(Wahyu_Katetreman),Dewa_Ruci,Wahyu_Makutharama,Kunthi_Pilih_(Lahiripun_Adipati_Karna),Sudamala,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Kartamarma</t>
@@ -2046,7 +2046,7 @@
     <t>Gusen</t>
   </si>
   <si>
-    <t>Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Wahyu_Makutharama,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Sudamala,Wahyu_Kaprawiran,Suksma_Langgeng,Wahyu_Cakraningrat,Wahyu_Kembar</t>
+    <t>Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Wahyu_Makutharama,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Sudamala,Wahyu_Kaprawiran,Suksma_Langgeng,Wahyu_Cakraningrat,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Kartapiyoga</t>
@@ -2118,7 +2118,7 @@
     <t>Surak</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Wahyu_Topeng_Waja,Dewa_Ruci,Semar_Mantu,Wahyu_Makutharama,Semar_mBangun_Kayangan,Basudewa_Grogol,Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Sudamala,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
+    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Wahyu_Topeng_Waja,Dewa_Ruci,Semar_Mantu,Wahyu_Makutharama,Semar_mBangun_Kayangan,Basudewa_Grogol,Prabu_Bimasakti,Sudamala,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Yuda_Kala_Kresna</t>
@@ -2547,7 +2547,7 @@
     <t>884-885</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Wahyu_Makutharama,Semar_mBangun_Kayangan,Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
+    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Wahyu_Makutharama,Semar_mBangun_Kayangan,Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Narada in Hindu mythology is known as a sage who is a /trilokasanjaari/ (the traveler of the three worlds: Heaven, Earth and the Underworld) as he is able to go to any of these three places at will. He is known as the son of Brahma. He said to have been cursed by Daksha his brother, to create conflict amongst people wherever he goes. However, the conflicts that he causes will be a blessing in disguise and lead to the greater good for the people. He is also considered to be a great devotee of Lord Vishnu.</t>
@@ -2767,7 +2767,7 @@
     <t>Songer, Dlonger</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Wahyu_Topeng_Waja,Semar_Mantu,Semar_Barang_Jantur,Semar_mBangun_Kayangan,Basudewa_Grogol,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Kunthi_Pilih_(Lahiripun_Adipati_Karna),Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Wahyu_Kembar</t>
+    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Wahyu_Topeng_Waja,Semar_Mantu,Semar_Barang_Jantur,Semar_mBangun_Kayangan,Basudewa_Grogol,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Prabu_Bimasakti,Kunthi_Pilih_(Lahiripun_Adipati_Karna),Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Pracona</t>
@@ -2925,7 +2925,7 @@
     <t>Nukma</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Wahyu_Makutharama,Semar_mBangun_Kayangan,Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Wahyu_Cakraningrat,Wahyu_Kembar</t>
+    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Wahyu_Makutharama,Semar_mBangun_Kayangan,Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Wahyu_Cakraningrat,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Prabu (Ramuwijaya) / Raden Ramaregawa</t>
@@ -3343,7 +3343,7 @@
     <t>Lintang, Dhunuk</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Wahyu_Topeng_Waja,Semar_Mantu,Semar_Barang_Jantur,Semar_mBangun_Kayangan,Basudewa_Grogol,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Kunthi_Pilih_(Lahiripun_Adipati_Karna),Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
+    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Wahyu_Topeng_Waja,Semar_Mantu,Semar_Barang_Jantur,Semar_mBangun_Kayangan,Basudewa_Grogol,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Prabu_Bimasakti,Kunthi_Pilih_(Lahiripun_Adipati_Karna),Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Bandung_Nagasewu,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Sengkuni</t>
@@ -3385,7 +3385,7 @@
     <t>1034-1037</t>
   </si>
   <si>
-    <t>Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Semar_Mantu,Wahyu_Makutharama,Semar_mBangun_Kayangan,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Kunthi_Pilih_(Lahiripun_Adipati_Karna),Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Wahyu_Cakraningrat,Wahyu_Kembar</t>
+    <t>Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Dewa_Ruci,Semar_Mantu,Wahyu_Makutharama,Semar_mBangun_Kayangan,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Prabu_Bimasakti,Kunthi_Pilih_(Lahiripun_Adipati_Karna),Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Wahyu_Cakraningrat,Wahyu_Kembar</t>
   </si>
   <si>
     <t>Setyaboma</t>
@@ -3805,7 +3805,7 @@
     <t>210-211 (Vol. IX)</t>
   </si>
   <si>
-    <t>Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Semar_Boyong_(Wahyu_Katentreman),Suksma_Langgeng</t>
+    <t>Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Suksma_Langgeng</t>
   </si>
   <si>
     <t>Known as Bhima, Hanuman's younger brother and the second Pandava.</t>
@@ -3852,7 +3852,7 @@
     <t>Lindhu</t>
   </si>
   <si>
-    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Wahyu_Topeng_Waja,Dewa_Ruci,Semar_Mantu,Wahyu_Makutharama,Semar_mBangun_Kayangan,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Semar_Boyong_(Wahyu_Katentreman),Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
+    <t>Narayana_Kridha_Brata,Wisanggeni_Lahir,Semar_Boyong_(Wahyu_Katetreman),Puntadewa_Wisudha,Wahyu_Topeng_Waja,Dewa_Ruci,Semar_Mantu,Wahyu_Makutharama,Semar_mBangun_Kayangan,Brajadhenta_Mbalela_(Gatotkaca_Wisudha),Prabu_Bimasakti,Sudamala,Babad_Wanamarta,Wahyu_Kaprawiran,Semar_Mantu_Alternative_Version,Suksma_Langgeng,Bandung_Nagasewu,Wahyu_Cakraningrat,Gatotkaca_Lahir,Wahyu_Kembar</t>
   </si>
   <si>
     <t xml:space="preserve">Vibisana is the younger brother of Ravana. In the Indian Ramayana, he is a giant, not a human. </t>

</xml_diff>